<commit_message>
In-progress manual adjustements to Adderbury1301, upload of meeting notes per V's request, restructuring of archive folder
</commit_message>
<xml_diff>
--- a/archive/Adderbury_1301_wl_format.xlsx
+++ b/archive/Adderbury_1301_wl_format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/victoriagierok/Dropbox/Physical Capital England/Decennial 2018/Detailed Estimates/Winchester Pipe Rolls/1301-1302/final new agricultural production/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubak\Documents\GitHub\student_assistant_manorial_records\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FAE186C6-620F-43DB-B681-1E50833A6C72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10482DBC-AC2A-47F3-B048-DDD0883A1910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="500" windowWidth="20220" windowHeight="16540" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="8715" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adderbury Overview" sheetId="13" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Issues of the Grange raw" sheetId="10" r:id="rId8"/>
     <sheet name="Sale of Corn Prices" sheetId="12" r:id="rId9"/>
     <sheet name="Prices" sheetId="7" r:id="rId10"/>
-    <sheet name="Labour Rents" sheetId="8" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="14" r:id="rId11"/>
+    <sheet name="Labour Rents" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -3505,21 +3506,21 @@
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F47" sqref="F47"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="78.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="78.26953125" style="80" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="80" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="80" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7265625" style="80" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="80" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" style="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.85546875" style="79" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.85546875" style="80"/>
+    <col min="5" max="5" width="20.1796875" style="80" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.81640625" style="79" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7265625" style="65" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.81640625" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -4874,7 +4875,7 @@
       </c>
       <c r="G76" s="94"/>
     </row>
-    <row r="77" spans="1:7" ht="17.100000000000001">
+    <row r="77" spans="1:7">
       <c r="A77" s="21" t="s">
         <v>84</v>
       </c>
@@ -4900,7 +4901,7 @@
       </c>
       <c r="G77" s="102"/>
     </row>
-    <row r="78" spans="1:7" ht="17.100000000000001">
+    <row r="78" spans="1:7">
       <c r="A78" s="21" t="s">
         <v>85</v>
       </c>
@@ -5395,7 +5396,7 @@
       <c r="G106" s="101"/>
       <c r="I106" s="98"/>
     </row>
-    <row r="107" spans="1:9" ht="17.100000000000001">
+    <row r="107" spans="1:9">
       <c r="A107" s="21" t="s">
         <v>111</v>
       </c>
@@ -5871,7 +5872,7 @@
       <c r="H139" s="95"/>
       <c r="I139" s="100"/>
     </row>
-    <row r="140" spans="1:9" ht="17.100000000000001">
+    <row r="140" spans="1:9">
       <c r="A140" s="21" t="s">
         <v>139</v>
       </c>
@@ -6207,14 +6208,14 @@
       <c r="G160" s="102"/>
       <c r="I160" s="98"/>
     </row>
-    <row r="161" spans="1:5" ht="17.100000000000001" thickBot="1">
+    <row r="161" spans="1:5" ht="16" thickBot="1">
       <c r="A161" s="2"/>
       <c r="B161" s="103"/>
       <c r="C161" s="98"/>
       <c r="D161" s="98"/>
       <c r="E161" s="98"/>
     </row>
-    <row r="162" spans="1:5" ht="17.100000000000001" thickBot="1">
+    <row r="162" spans="1:5" ht="16" thickBot="1">
       <c r="A162" s="75"/>
       <c r="B162" s="76" t="s">
         <v>4</v>
@@ -6309,7 +6310,7 @@
       <c r="D170" s="98"/>
       <c r="E170" s="111"/>
     </row>
-    <row r="171" spans="1:5" ht="17.100000000000001" thickBot="1">
+    <row r="171" spans="1:5" ht="16" thickBot="1">
       <c r="A171" s="85" t="s">
         <v>159</v>
       </c>
@@ -6335,19 +6336,31 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEB4B400-D94B-4343-A2DC-D1A1DF6D36D5}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6361,14 +6374,14 @@
       <selection activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="8.85546875" style="7"/>
-    <col min="6" max="6" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="255.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="7"/>
+    <col min="1" max="1" width="38.26953125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="8.81640625" style="7"/>
+    <col min="6" max="6" width="12.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="255.81640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8197,34 +8210,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="26" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="48.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7265625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="48.1796875" customWidth="1"/>
     <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" customWidth="1"/>
+    <col min="11" max="11" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.95">
+    <row r="1" spans="1:11" ht="15.5">
       <c r="A1" s="5" t="s">
         <v>257</v>
       </c>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:11" s="7" customFormat="1" ht="33.950000000000003">
+    <row r="2" spans="1:11" s="7" customFormat="1" ht="31">
       <c r="A2" s="8" t="s">
         <v>161</v>
       </c>
@@ -10420,7 +10433,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="15.95">
+    <row r="112" spans="1:8" ht="15.5">
       <c r="A112" s="4" t="s">
         <v>366</v>
       </c>
@@ -10445,7 +10458,7 @@
         <v>15.64</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="15.95">
+    <row r="113" spans="1:6" ht="15.5">
       <c r="A113" s="4" t="s">
         <v>367</v>
       </c>
@@ -10454,7 +10467,7 @@
         <v>16.177499999999998</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="15.95">
+    <row r="114" spans="1:6" ht="15.5">
       <c r="A114" s="4" t="s">
         <v>42</v>
       </c>
@@ -10463,7 +10476,7 @@
         <v>4.0474999999999994</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="15.95">
+    <row r="115" spans="1:6" ht="15.5">
       <c r="A115" s="4" t="s">
         <v>43</v>
       </c>
@@ -10472,7 +10485,7 @@
         <v>4.0474999999999994</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="15.95">
+    <row r="116" spans="1:6" ht="15.5">
       <c r="A116" s="98"/>
     </row>
   </sheetData>
@@ -10486,30 +10499,30 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="Q13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
       <selection pane="bottomRight" activeCell="X11" sqref="X11"/>
-      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="30.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.81640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="30.81640625" style="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -10872,7 +10885,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="9" spans="1:18" s="46" customFormat="1" ht="15.95">
+    <row r="9" spans="1:18" s="46" customFormat="1" ht="15.5">
       <c r="A9" s="46" t="s">
         <v>385</v>
       </c>
@@ -10900,7 +10913,7 @@
       <c r="N11" s="28"/>
       <c r="O11" s="28"/>
     </row>
-    <row r="12" spans="1:18" s="27" customFormat="1" ht="48">
+    <row r="12" spans="1:18" s="27" customFormat="1" ht="43.5">
       <c r="A12" s="27" t="s">
         <v>386</v>
       </c>
@@ -11209,7 +11222,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -11227,31 +11240,31 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="V80" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="V69" sqref="V69"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" style="32" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" style="32" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.42578125" style="32" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.28515625" style="32" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="61" customWidth="1"/>
-    <col min="13" max="13" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" style="28"/>
-    <col min="22" max="23" width="24.140625" style="28" customWidth="1"/>
-    <col min="24" max="24" width="8.85546875" style="28"/>
+    <col min="6" max="6" width="7.26953125" style="32" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.26953125" style="32" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.453125" style="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.26953125" style="32" customWidth="1"/>
+    <col min="10" max="10" width="10.7265625" style="32" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1796875" style="61" customWidth="1"/>
+    <col min="13" max="13" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.81640625" style="28"/>
+    <col min="22" max="23" width="24.1796875" style="28" customWidth="1"/>
+    <col min="24" max="24" width="8.81640625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="54" customFormat="1" ht="48">
+    <row r="1" spans="1:25" s="54" customFormat="1" ht="42">
       <c r="A1" s="52" t="s">
         <v>161</v>
       </c>
@@ -13538,19 +13551,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="H260" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="H65" sqref="H65"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.42578125" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.453125" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -26737,45 +26750,45 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AE50" sqref="AE50"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="102.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.453125" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.26953125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="10" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="8.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36">
@@ -32799,34 +32812,34 @@
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="80.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="80.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="31" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="29.81640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="33.7265625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
Progress in manual adjustements to overview sheets & meeting notes Sandra 31/10/25
</commit_message>
<xml_diff>
--- a/archive/Adderbury_1301_wl_format.xlsx
+++ b/archive/Adderbury_1301_wl_format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubak\Documents\GitHub\student_assistant_manorial_records\archive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10482DBC-AC2A-47F3-B048-DDD0883A1910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE5A7AD-183B-44C5-924F-495931F5371A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="8715" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5640" windowWidth="19360" windowHeight="10480" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Adderbury Overview" sheetId="13" r:id="rId1"/>
@@ -8210,8 +8210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="G38" sqref="G38"/>
@@ -9099,7 +9099,7 @@
         <v>0.97</v>
       </c>
       <c r="G38" s="26">
-        <v>1.0000000000000011E-2</v>
+        <v>0.01</v>
       </c>
       <c r="H38" t="s">
         <v>109</v>
@@ -10497,7 +10497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="12" topLeftCell="Q13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>

</xml_diff>